<commit_message>
Misc ODK-X form fixes
</commit_message>
<xml_diff>
--- a/odkx/forms/hh_geo_location.xlsx
+++ b/odkx/forms/hh_geo_location.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="initial" sheetId="1" state="visible" r:id="rId2"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="52">
   <si>
     <t xml:space="preserve">clause</t>
   </si>
@@ -45,6 +45,9 @@
   </si>
   <si>
     <t xml:space="preserve">name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">required</t>
   </si>
   <si>
     <t xml:space="preserve">display.prompt.text</t>
@@ -264,11 +267,11 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -295,26 +298,26 @@
       <selection pane="topLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.578125" defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.5859375" defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="0" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="0" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="s">
+      <c r="A2" s="1" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="s">
+      <c r="A3" s="1" t="s">
         <v>4</v>
       </c>
     </row>
@@ -334,49 +337,56 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E2"/>
+  <dimension ref="A1:F2"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C10" activeCellId="0" sqref="C10"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.578125" defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.5859375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="8.9"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="16"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="74.5"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="8.9"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="8.9"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="16"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="8.87"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="74.5"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="8.9"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="s">
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="0" t="s">
+      <c r="B1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C1" s="0" t="s">
+      <c r="C1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D1" s="0" t="s">
+      <c r="D1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="E1" s="0" t="s">
+      <c r="E1" s="1" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="2" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B2" s="1" t="s">
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="B2" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="E2" s="0" t="s">
+      <c r="C2" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="D2" s="2" t="s">
         <v>13</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>14</v>
       </c>
     </row>
   </sheetData>
@@ -397,138 +407,126 @@
   </sheetPr>
   <dimension ref="A1:H8"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.578125" defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.5859375" defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="13.33"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="16.03"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="16.97"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="19.78"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="20.37"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="18.72"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="21.55"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="22.13"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="13.33"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="16.03"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="16.97"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="19.78"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="20.37"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="18.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="21.55"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="22.13"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="s">
-        <v>14</v>
-      </c>
-      <c r="B1" s="0" t="s">
+      <c r="A1" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="B1" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="C1" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="D1" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="E1" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="F1" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="G1" s="1" t="s">
         <v>21</v>
       </c>
+      <c r="H1" s="1" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="s">
-        <v>22</v>
-      </c>
-      <c r="B2" s="0" t="s">
-        <v>11</v>
+      <c r="A2" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="s">
-        <v>23</v>
-      </c>
-      <c r="B3" s="0" t="n">
+      <c r="A3" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B3" s="1" t="n">
         <v>20210109001</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="s">
-        <v>24</v>
-      </c>
-      <c r="B4" s="0" t="s">
-        <v>11</v>
+      <c r="A4" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="0" t="s">
-        <v>25</v>
-      </c>
-      <c r="C5" s="0" t="s">
+      <c r="A5" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="D5" s="0" t="s">
-        <v>26</v>
-      </c>
-      <c r="E5" s="0" t="s">
-        <v>26</v>
+      <c r="C5" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="B6" s="2"/>
-      <c r="C6" s="2"/>
-      <c r="D6" s="2"/>
-      <c r="E6" s="2"/>
-      <c r="F6" s="2" t="s">
+      <c r="A6" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="G6" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="H6" s="2" t="s">
-        <v>28</v>
+      <c r="F6" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="H6" s="1" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="B7" s="2"/>
-      <c r="C7" s="2"/>
-      <c r="D7" s="2"/>
-      <c r="E7" s="2"/>
-      <c r="F7" s="2" t="s">
+      <c r="A7" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="G7" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="H7" s="2" t="s">
-        <v>30</v>
+      <c r="F7" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="H7" s="1" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="B8" s="2"/>
-      <c r="C8" s="2"/>
-      <c r="D8" s="2"/>
-      <c r="E8" s="2"/>
-      <c r="F8" s="2" t="s">
+      <c r="A8" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="G8" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="H8" s="2" t="s">
-        <v>32</v>
+      <c r="F8" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="G8" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="H8" s="1" t="s">
+        <v>33</v>
       </c>
     </row>
   </sheetData>
@@ -553,114 +551,114 @@
       <selection pane="topLeft" activeCell="E3" activeCellId="0" sqref="E3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.578125" defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.5859375" defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="17.1"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="17.1"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="62.2"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="17.1"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="17.1"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="62.21"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="s">
-        <v>33</v>
-      </c>
-      <c r="B1" s="0" t="s">
+      <c r="A1" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="C1" s="0" t="s">
+      <c r="B1" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="D1" s="0" t="s">
+      <c r="C1" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="E1" s="0" t="s">
-        <v>15</v>
+      <c r="E1" s="1" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="s">
-        <v>36</v>
-      </c>
-      <c r="B2" s="0" t="s">
-        <v>27</v>
-      </c>
-      <c r="C2" s="0" t="s">
+      <c r="A2" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="D2" s="0" t="s">
+      <c r="B2" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C2" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="E2" s="0" t="s">
+      <c r="D2" s="1" t="s">
         <v>39</v>
       </c>
+      <c r="E2" s="1" t="s">
+        <v>40</v>
+      </c>
     </row>
     <row r="3" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="s">
-        <v>36</v>
-      </c>
-      <c r="B3" s="0" t="s">
-        <v>27</v>
-      </c>
-      <c r="C3" s="0" t="s">
-        <v>40</v>
-      </c>
-      <c r="D3" s="0" t="s">
+      <c r="A3" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C3" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="E3" s="0" t="s">
+      <c r="D3" s="1" t="s">
         <v>42</v>
       </c>
+      <c r="E3" s="1" t="s">
+        <v>43</v>
+      </c>
     </row>
     <row r="4" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="s">
-        <v>43</v>
-      </c>
-      <c r="B4" s="0" t="s">
-        <v>27</v>
-      </c>
-      <c r="C4" s="0" t="s">
+      <c r="A4" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="D4" s="0" t="s">
-        <v>41</v>
-      </c>
-      <c r="E4" s="0" t="s">
+      <c r="B4" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C4" s="1" t="s">
         <v>45</v>
       </c>
+      <c r="D4" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>46</v>
+      </c>
     </row>
     <row r="5" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="0" t="s">
-        <v>43</v>
-      </c>
-      <c r="B5" s="0" t="s">
-        <v>27</v>
-      </c>
-      <c r="C5" s="0" t="s">
-        <v>46</v>
-      </c>
-      <c r="D5" s="0" t="s">
-        <v>41</v>
-      </c>
-      <c r="E5" s="0" t="s">
+      <c r="A5" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C5" s="1" t="s">
         <v>47</v>
       </c>
+      <c r="D5" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>48</v>
+      </c>
     </row>
     <row r="6" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="0" t="s">
-        <v>43</v>
-      </c>
-      <c r="B6" s="0" t="s">
-        <v>27</v>
-      </c>
-      <c r="C6" s="0" t="s">
-        <v>48</v>
-      </c>
-      <c r="D6" s="0" t="s">
-        <v>41</v>
-      </c>
-      <c r="E6" s="0" t="s">
+      <c r="A6" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C6" s="1" t="s">
         <v>49</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>50</v>
       </c>
     </row>
   </sheetData>
@@ -685,33 +683,33 @@
       <selection pane="topLeft" activeCell="C1" activeCellId="0" sqref="C1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.578125" defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.5859375" defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="26.3"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="26.3"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="s">
+      <c r="A1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B1" s="0" t="s">
+      <c r="B1" s="1" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="s">
-        <v>50</v>
-      </c>
-      <c r="B2" s="0" t="s">
-        <v>41</v>
+      <c r="A2" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="1" t="s">
+      <c r="A3" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B3" s="1" t="s">
         <v>11</v>
-      </c>
-      <c r="B3" s="0" t="s">
-        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>